<commit_message>
Update UI Appframework 3
</commit_message>
<xml_diff>
--- a/document/技术详细设计.xlsx
+++ b/document/技术详细设计.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Node.js" sheetId="2" r:id="rId1"/>
@@ -81,23 +81,23 @@
     <t xml:space="preserve">Web server </t>
   </si>
   <si>
-    <t>1. All username should be encrypted by DES</t>
-  </si>
-  <si>
-    <t>2. All password should be encrypted by MD5</t>
-  </si>
-  <si>
     <t>7. if the key is saved in database, it will have additonal "_db" at the tail when being sent back (in DB, no additonal words there)</t>
   </si>
   <si>
     <t>8. If the key is saved in memory, "_me" will be added as the same</t>
+  </si>
+  <si>
+    <t>http://www.w3cplus.com/content/css3-font-face</t>
+  </si>
+  <si>
+    <t>https://icomoon.io/app/#/select</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +109,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -131,17 +139,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -528,7 +539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="H22" sqref="H22:H23"/>
     </sheetView>
   </sheetViews>
@@ -566,12 +577,12 @@
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -581,25 +592,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:B5"/>
+  <dimension ref="A2:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>22</v>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2" location="/select"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>